<commit_message>
Adding real counts data
</commit_message>
<xml_diff>
--- a/output/sites/test_differences_nut_scenarios_CN.xlsx
+++ b/output/sites/test_differences_nut_scenarios_CN.xlsx
@@ -446,22 +446,22 @@
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>0.008</v>
+        <v>0.004</v>
       </c>
       <c r="E2" t="n">
-        <v>0.829</v>
+        <v>0.834</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.006</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="3">
@@ -475,22 +475,22 @@
         <v>11</v>
       </c>
       <c r="D3" t="n">
-        <v>0.018</v>
+        <v>0.007</v>
       </c>
       <c r="E3" t="n">
-        <v>0.784</v>
+        <v>0.795</v>
       </c>
       <c r="F3" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
       <c r="G3" t="n">
         <v>0.005</v>
       </c>
       <c r="H3" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
       <c r="I3" t="n">
-        <v>0.013</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="4">
@@ -504,22 +504,22 @@
         <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>0.041</v>
+        <v>0.024</v>
       </c>
       <c r="E4" t="n">
-        <v>0.739</v>
+        <v>0.764</v>
       </c>
       <c r="F4" t="n">
-        <v>0.016</v>
+        <v>0.003</v>
       </c>
       <c r="G4" t="n">
-        <v>0.018</v>
+        <v>0.012</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01</v>
+        <v>0.008</v>
       </c>
       <c r="I4" t="n">
-        <v>0.029</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="5">
@@ -533,22 +533,22 @@
         <v>13</v>
       </c>
       <c r="D5" t="n">
-        <v>0.095</v>
+        <v>0.064</v>
       </c>
       <c r="E5" t="n">
-        <v>0.68</v>
+        <v>0.702</v>
       </c>
       <c r="F5" t="n">
-        <v>0.049</v>
+        <v>0.022</v>
       </c>
       <c r="G5" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.057</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.046</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.091</v>
       </c>
     </row>
     <row r="6">
@@ -562,22 +562,22 @@
         <v>14</v>
       </c>
       <c r="D6" t="n">
-        <v>0.231</v>
+        <v>0.22</v>
       </c>
       <c r="E6" t="n">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
       <c r="F6" t="n">
-        <v>0.185</v>
+        <v>0.155</v>
       </c>
       <c r="G6" t="n">
-        <v>0.195</v>
+        <v>0.179</v>
       </c>
       <c r="H6" t="n">
         <v>0.163</v>
       </c>
       <c r="I6" t="n">
-        <v>0.231</v>
+        <v>0.214</v>
       </c>
     </row>
     <row r="7">
@@ -591,22 +591,22 @@
         <v>15</v>
       </c>
       <c r="D7" t="n">
-        <v>0.515</v>
+        <v>0.523</v>
       </c>
       <c r="E7" t="n">
-        <v>0.495</v>
+        <v>0.493</v>
       </c>
       <c r="F7" t="n">
-        <v>0.52</v>
+        <v>0.472</v>
       </c>
       <c r="G7" t="n">
-        <v>0.497</v>
+        <v>0.506</v>
       </c>
       <c r="H7" t="n">
-        <v>0.502</v>
+        <v>0.5</v>
       </c>
       <c r="I7" t="n">
-        <v>0.509</v>
+        <v>0.538</v>
       </c>
     </row>
     <row r="8">
@@ -620,22 +620,22 @@
         <v>16</v>
       </c>
       <c r="D8" t="n">
-        <v>0.85</v>
+        <v>0.852</v>
       </c>
       <c r="E8" t="n">
-        <v>0.398</v>
+        <v>0.37</v>
       </c>
       <c r="F8" t="n">
-        <v>0.876</v>
+        <v>0.902</v>
       </c>
       <c r="G8" t="n">
-        <v>0.869</v>
+        <v>0.882</v>
       </c>
       <c r="H8" t="n">
+        <v>0.892</v>
+      </c>
+      <c r="I8" t="n">
         <v>0.868</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.857</v>
       </c>
     </row>
     <row r="9">
@@ -649,22 +649,22 @@
         <v>17</v>
       </c>
       <c r="D9" t="n">
-        <v>0.991</v>
+        <v>0.995</v>
       </c>
       <c r="E9" t="n">
-        <v>0.236</v>
+        <v>0.214</v>
       </c>
       <c r="F9" t="n">
-        <v>0.995</v>
+        <v>0.998</v>
       </c>
       <c r="G9" t="n">
-        <v>0.996</v>
+        <v>0.998</v>
       </c>
       <c r="H9" t="n">
-        <v>0.997</v>
+        <v>0.998</v>
       </c>
       <c r="I9" t="n">
-        <v>0.993</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="10">
@@ -681,7 +681,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.09</v>
+        <v>0.078</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -710,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0.019</v>
+        <v>0.007</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
@@ -768,16 +768,16 @@
         <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>0.539</v>
+        <v>0.493</v>
       </c>
       <c r="F13" t="n">
-        <v>0.823</v>
+        <v>0.841</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>0.035</v>
+        <v>0.021</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
@@ -797,16 +797,16 @@
         <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>0.529</v>
+        <v>0.531</v>
       </c>
       <c r="F14" t="n">
-        <v>0.792</v>
+        <v>0.818</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>0.037</v>
+        <v>0.047</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
@@ -829,13 +829,13 @@
         <v>0.518</v>
       </c>
       <c r="F15" t="n">
-        <v>0.745</v>
+        <v>0.752</v>
       </c>
       <c r="G15" t="n">
         <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>0.086</v>
+        <v>0.064</v>
       </c>
       <c r="I15" t="n">
         <v>1</v>
@@ -855,16 +855,16 @@
         <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>0.505</v>
+        <v>0.522</v>
       </c>
       <c r="F16" t="n">
-        <v>0.668</v>
+        <v>0.694</v>
       </c>
       <c r="G16" t="n">
         <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>0.179</v>
+        <v>0.162</v>
       </c>
       <c r="I16" t="n">
         <v>1</v>
@@ -881,22 +881,22 @@
         <v>14</v>
       </c>
       <c r="D17" t="n">
-        <v>0.993</v>
+        <v>0.997</v>
       </c>
       <c r="E17" t="n">
-        <v>0.484</v>
+        <v>0.501</v>
       </c>
       <c r="F17" t="n">
-        <v>0.597</v>
+        <v>0.62</v>
       </c>
       <c r="G17" t="n">
-        <v>0.968</v>
+        <v>0.98</v>
       </c>
       <c r="H17" t="n">
-        <v>0.306</v>
+        <v>0.273</v>
       </c>
       <c r="I17" t="n">
-        <v>0.991</v>
+        <v>0.994</v>
       </c>
     </row>
     <row r="18">
@@ -910,22 +910,22 @@
         <v>15</v>
       </c>
       <c r="D18" t="n">
-        <v>0.512</v>
+        <v>0.513</v>
       </c>
       <c r="E18" t="n">
-        <v>0.527</v>
+        <v>0.511</v>
       </c>
       <c r="F18" t="n">
-        <v>0.526</v>
+        <v>0.483</v>
       </c>
       <c r="G18" t="n">
-        <v>0.519</v>
+        <v>0.493</v>
       </c>
       <c r="H18" t="n">
-        <v>0.487</v>
+        <v>0.484</v>
       </c>
       <c r="I18" t="n">
-        <v>0.504</v>
+        <v>0.521</v>
       </c>
     </row>
     <row r="19">
@@ -939,22 +939,22 @@
         <v>16</v>
       </c>
       <c r="D19" t="n">
-        <v>0.013</v>
+        <v>0.003</v>
       </c>
       <c r="E19" t="n">
-        <v>0.489</v>
+        <v>0.49</v>
       </c>
       <c r="F19" t="n">
-        <v>0.413</v>
+        <v>0.383</v>
       </c>
       <c r="G19" t="n">
-        <v>0.02</v>
+        <v>0.022</v>
       </c>
       <c r="H19" t="n">
-        <v>0.748</v>
+        <v>0.749</v>
       </c>
       <c r="I19" t="n">
-        <v>0.014</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="20">
@@ -971,16 +971,16 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.477</v>
+        <v>0.475</v>
       </c>
       <c r="F20" t="n">
-        <v>0.296</v>
+        <v>0.27</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>0.914</v>
+        <v>0.939</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -1000,16 +1000,16 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.474</v>
+        <v>0.455</v>
       </c>
       <c r="F21" t="n">
-        <v>0.208</v>
+        <v>0.158</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>0.992</v>
+        <v>0.994</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
@@ -1029,10 +1029,10 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0.466</v>
+        <v>0.452</v>
       </c>
       <c r="F22" t="n">
-        <v>0.108</v>
+        <v>0.069</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
@@ -1058,10 +1058,10 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0.448</v>
+        <v>0.416</v>
       </c>
       <c r="F23" t="n">
-        <v>0.041</v>
+        <v>0.025</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -1084,22 +1084,22 @@
         <v>10</v>
       </c>
       <c r="D24" t="n">
-        <v>0.003</v>
+        <v>0.006</v>
       </c>
       <c r="E24" t="n">
-        <v>0.998</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
-        <v>0.791</v>
+        <v>0.805</v>
       </c>
       <c r="G24" t="n">
-        <v>0.375</v>
+        <v>0.39</v>
       </c>
       <c r="H24" t="n">
-        <v>0.625</v>
+        <v>0.614</v>
       </c>
       <c r="I24" t="n">
-        <v>0.013</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="25">
@@ -1113,22 +1113,22 @@
         <v>11</v>
       </c>
       <c r="D25" t="n">
-        <v>0.017</v>
+        <v>0.01</v>
       </c>
       <c r="E25" t="n">
-        <v>0.993</v>
+        <v>0.992</v>
       </c>
       <c r="F25" t="n">
-        <v>0.753</v>
+        <v>0.772</v>
       </c>
       <c r="G25" t="n">
-        <v>0.413</v>
+        <v>0.395</v>
       </c>
       <c r="H25" t="n">
-        <v>0.608</v>
+        <v>0.588</v>
       </c>
       <c r="I25" t="n">
-        <v>0.032</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="26">
@@ -1142,22 +1142,22 @@
         <v>12</v>
       </c>
       <c r="D26" t="n">
-        <v>0.032</v>
+        <v>0.028</v>
       </c>
       <c r="E26" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="F26" t="n">
-        <v>0.721</v>
+        <v>0.728</v>
       </c>
       <c r="G26" t="n">
         <v>0.411</v>
       </c>
       <c r="H26" t="n">
-        <v>0.551</v>
+        <v>0.591</v>
       </c>
       <c r="I26" t="n">
-        <v>0.06</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="27">
@@ -1171,22 +1171,22 @@
         <v>13</v>
       </c>
       <c r="D27" t="n">
-        <v>0.096</v>
+        <v>0.085</v>
       </c>
       <c r="E27" t="n">
-        <v>0.922</v>
+        <v>0.928</v>
       </c>
       <c r="F27" t="n">
-        <v>0.632</v>
+        <v>0.681</v>
       </c>
       <c r="G27" t="n">
-        <v>0.454</v>
+        <v>0.433</v>
       </c>
       <c r="H27" t="n">
-        <v>0.545</v>
+        <v>0.583</v>
       </c>
       <c r="I27" t="n">
-        <v>0.122</v>
+        <v>0.109</v>
       </c>
     </row>
     <row r="28">
@@ -1200,22 +1200,22 @@
         <v>14</v>
       </c>
       <c r="D28" t="n">
-        <v>0.264</v>
+        <v>0.225</v>
       </c>
       <c r="E28" t="n">
-        <v>0.757</v>
+        <v>0.758</v>
       </c>
       <c r="F28" t="n">
-        <v>0.585</v>
+        <v>0.576</v>
       </c>
       <c r="G28" t="n">
-        <v>0.468</v>
+        <v>0.464</v>
       </c>
       <c r="H28" t="n">
-        <v>0.543</v>
+        <v>0.567</v>
       </c>
       <c r="I28" t="n">
-        <v>0.291</v>
+        <v>0.255</v>
       </c>
     </row>
     <row r="29">
@@ -1229,22 +1229,22 @@
         <v>15</v>
       </c>
       <c r="D29" t="n">
-        <v>0.51</v>
+        <v>0.528</v>
       </c>
       <c r="E29" t="n">
-        <v>0.51</v>
+        <v>0.486</v>
       </c>
       <c r="F29" t="n">
-        <v>0.509</v>
+        <v>0.496</v>
       </c>
       <c r="G29" t="n">
-        <v>0.509</v>
+        <v>0.497</v>
       </c>
       <c r="H29" t="n">
-        <v>0.483</v>
+        <v>0.496</v>
       </c>
       <c r="I29" t="n">
-        <v>0.523</v>
+        <v>0.529</v>
       </c>
     </row>
     <row r="30">
@@ -1258,22 +1258,22 @@
         <v>16</v>
       </c>
       <c r="D30" t="n">
-        <v>0.813</v>
+        <v>0.839</v>
       </c>
       <c r="E30" t="n">
-        <v>0.207</v>
+        <v>0.18</v>
       </c>
       <c r="F30" t="n">
-        <v>0.443</v>
+        <v>0.382</v>
       </c>
       <c r="G30" t="n">
-        <v>0.544</v>
+        <v>0.553</v>
       </c>
       <c r="H30" t="n">
-        <v>0.454</v>
+        <v>0.445</v>
       </c>
       <c r="I30" t="n">
-        <v>0.781</v>
+        <v>0.793</v>
       </c>
     </row>
     <row r="31">
@@ -1287,22 +1287,22 @@
         <v>17</v>
       </c>
       <c r="D31" t="n">
-        <v>0.968</v>
+        <v>0.983</v>
       </c>
       <c r="E31" t="n">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="F31" t="n">
-        <v>0.311</v>
+        <v>0.29</v>
       </c>
       <c r="G31" t="n">
-        <v>0.587</v>
+        <v>0.584</v>
       </c>
       <c r="H31" t="n">
-        <v>0.406</v>
+        <v>0.412</v>
       </c>
       <c r="I31" t="n">
-        <v>0.945</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="32">
@@ -1316,22 +1316,22 @@
         <v>18</v>
       </c>
       <c r="D32" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.162</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.646</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="I32" t="n">
         <v>0.999</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="F32" t="n">
-        <v>0.198</v>
-      </c>
-      <c r="G32" t="n">
-        <v>0.634</v>
-      </c>
-      <c r="H32" t="n">
-        <v>0.347</v>
-      </c>
-      <c r="I32" t="n">
-        <v>0.996</v>
       </c>
     </row>
     <row r="33">
@@ -1351,13 +1351,13 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0.11</v>
+        <v>0.099</v>
       </c>
       <c r="G33" t="n">
-        <v>0.704</v>
+        <v>0.7</v>
       </c>
       <c r="H33" t="n">
-        <v>0.288</v>
+        <v>0.289</v>
       </c>
       <c r="I33" t="n">
         <v>1</v>
@@ -1380,13 +1380,13 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.044</v>
+        <v>0.032</v>
       </c>
       <c r="G34" t="n">
-        <v>0.75</v>
+        <v>0.795</v>
       </c>
       <c r="H34" t="n">
-        <v>0.212</v>
+        <v>0.187</v>
       </c>
       <c r="I34" t="n">
         <v>1</v>
@@ -1406,19 +1406,19 @@
         <v>0.022</v>
       </c>
       <c r="E35" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F35" t="n">
-        <v>0.954</v>
+        <v>0.975</v>
       </c>
       <c r="G35" t="n">
-        <v>0.008</v>
+        <v>0.006</v>
       </c>
       <c r="H35" t="n">
         <v>1</v>
       </c>
       <c r="I35" t="n">
-        <v>0.024</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="36">
@@ -1432,22 +1432,22 @@
         <v>11</v>
       </c>
       <c r="D36" t="n">
-        <v>0.038</v>
+        <v>0.021</v>
       </c>
       <c r="E36" t="n">
-        <v>0.006</v>
+        <v>0.001</v>
       </c>
       <c r="F36" t="n">
-        <v>0.932</v>
+        <v>0.959</v>
       </c>
       <c r="G36" t="n">
-        <v>0.022</v>
+        <v>0.01</v>
       </c>
       <c r="H36" t="n">
         <v>1</v>
       </c>
       <c r="I36" t="n">
-        <v>0.037</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="37">
@@ -1461,22 +1461,22 @@
         <v>12</v>
       </c>
       <c r="D37" t="n">
-        <v>0.079</v>
+        <v>0.075</v>
       </c>
       <c r="E37" t="n">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="F37" t="n">
-        <v>0.902</v>
+        <v>0.924</v>
       </c>
       <c r="G37" t="n">
-        <v>0.044</v>
+        <v>0.029</v>
       </c>
       <c r="H37" t="n">
         <v>1</v>
       </c>
       <c r="I37" t="n">
-        <v>0.073</v>
+        <v>0.063</v>
       </c>
     </row>
     <row r="38">
@@ -1490,22 +1490,22 @@
         <v>13</v>
       </c>
       <c r="D38" t="n">
-        <v>0.147</v>
+        <v>0.112</v>
       </c>
       <c r="E38" t="n">
-        <v>0.055</v>
+        <v>0.03</v>
       </c>
       <c r="F38" t="n">
-        <v>0.804</v>
+        <v>0.854</v>
       </c>
       <c r="G38" t="n">
-        <v>0.098</v>
+        <v>0.066</v>
       </c>
       <c r="H38" t="n">
-        <v>0.995</v>
+        <v>0.999</v>
       </c>
       <c r="I38" t="n">
-        <v>0.146</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="39">
@@ -1519,22 +1519,22 @@
         <v>14</v>
       </c>
       <c r="D39" t="n">
-        <v>0.288</v>
+        <v>0.255</v>
       </c>
       <c r="E39" t="n">
-        <v>0.178</v>
+        <v>0.136</v>
       </c>
       <c r="F39" t="n">
-        <v>0.693</v>
+        <v>0.709</v>
       </c>
       <c r="G39" t="n">
-        <v>0.245</v>
+        <v>0.191</v>
       </c>
       <c r="H39" t="n">
-        <v>0.91</v>
+        <v>0.935</v>
       </c>
       <c r="I39" t="n">
-        <v>0.285</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="40">
@@ -1548,22 +1548,22 @@
         <v>15</v>
       </c>
       <c r="D40" t="n">
-        <v>0.505</v>
+        <v>0.496</v>
       </c>
       <c r="E40" t="n">
-        <v>0.527</v>
+        <v>0.491</v>
       </c>
       <c r="F40" t="n">
-        <v>0.488</v>
+        <v>0.481</v>
       </c>
       <c r="G40" t="n">
+        <v>0.497</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.517</v>
+      </c>
+      <c r="I40" t="n">
         <v>0.506</v>
-      </c>
-      <c r="H40" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="I40" t="n">
-        <v>0.505</v>
       </c>
     </row>
     <row r="41">
@@ -1577,22 +1577,22 @@
         <v>16</v>
       </c>
       <c r="D41" t="n">
-        <v>0.816</v>
+        <v>0.819</v>
       </c>
       <c r="E41" t="n">
-        <v>0.905</v>
+        <v>0.906</v>
       </c>
       <c r="F41" t="n">
-        <v>0.256</v>
+        <v>0.213</v>
       </c>
       <c r="G41" t="n">
-        <v>0.855</v>
+        <v>0.866</v>
       </c>
       <c r="H41" t="n">
-        <v>0.045</v>
+        <v>0.025</v>
       </c>
       <c r="I41" t="n">
-        <v>0.811</v>
+        <v>0.831</v>
       </c>
     </row>
     <row r="42">
@@ -1606,22 +1606,22 @@
         <v>17</v>
       </c>
       <c r="D42" t="n">
-        <v>0.971</v>
+        <v>0.981</v>
       </c>
       <c r="E42" t="n">
-        <v>0.998</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
-        <v>0.064</v>
+        <v>0.033</v>
       </c>
       <c r="G42" t="n">
-        <v>0.991</v>
+        <v>0.994</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>0.969</v>
+        <v>0.984</v>
       </c>
     </row>
     <row r="43">
@@ -1641,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="F43" t="n">
-        <v>0.004</v>
+        <v>0</v>
       </c>
       <c r="G43" t="n">
         <v>1</v>

</xml_diff>